<commit_message>
datos bajados por ema
</commit_message>
<xml_diff>
--- a/datos/multiparametricas.xlsx
+++ b/datos/multiparametricas.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="multiparametricas" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Muestreo RNUO" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="76">
   <si>
     <t xml:space="preserve">Referencias Equipos</t>
   </si>
@@ -209,6 +210,45 @@
   </si>
   <si>
     <t xml:space="preserve">24.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fecha:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24/02/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muestra:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUFFER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hora:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atlas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muni 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muni 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alcantarilla 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alcantarilla 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESERVORIO</t>
   </si>
 </sst>
 </file>
@@ -219,11 +259,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -240,6 +281,19 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -249,12 +303,33 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -283,12 +358,56 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -305,283 +424,786 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R10" activeCellId="0" sqref="R10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="6.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="6.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="7.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="6.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="6.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="9.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="5.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="6.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="1" width="6.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="6.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="7.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="6.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="6.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="9.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="5.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="1" width="6.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="L8" s="0" t="s">
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O8" s="0" t="s">
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="G9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="0" t="s">
+      <c r="H9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="0" t="s">
+      <c r="I9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="0" t="s">
+      <c r="J9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K9" s="0" t="s">
+      <c r="K9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L9" s="0" t="s">
+      <c r="L9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M9" s="0" t="s">
+      <c r="M9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="N9" s="0" t="s">
+      <c r="N9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O9" s="0" t="s">
+      <c r="O9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="P9" s="0" t="s">
+      <c r="P9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q9" s="0" t="s">
+      <c r="Q9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="R9" s="0" t="s">
+      <c r="R9" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J10" s="0" t="s">
+      <c r="J10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K10" s="0" t="s">
+      <c r="K10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L10" s="0" t="s">
+      <c r="L10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="N10" s="0" t="s">
+      <c r="N10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="O10" s="0" t="s">
+      <c r="O10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="P10" s="0" t="s">
+      <c r="P10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="Q10" s="0" t="s">
+      <c r="Q10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="R10" s="0" t="s">
+      <c r="R10" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I11" s="0" t="s">
+      <c r="I11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J11" s="0" t="s">
+      <c r="J11" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="K11" s="0" t="n">
+      <c r="K11" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="L11" s="0" t="s">
+      <c r="L11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="N11" s="0" t="n">
+      <c r="N11" s="1" t="n">
         <v>752</v>
       </c>
-      <c r="O11" s="0" t="s">
+      <c r="O11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="P11" s="0" t="n">
+      <c r="P11" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="Q11" s="0" t="s">
+      <c r="Q11" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="R11" s="0" t="s">
+      <c r="R11" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12" s="1" t="n">
         <v>86</v>
       </c>
-      <c r="I12" s="0" t="s">
+      <c r="I12" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="J12" s="0" t="s">
+      <c r="J12" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="K12" s="0" t="s">
+      <c r="K12" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="L12" s="0" t="n">
+      <c r="L12" s="1" t="n">
         <v>3161</v>
       </c>
-      <c r="N12" s="0" t="n">
+      <c r="N12" s="1" t="n">
         <v>3175</v>
       </c>
-      <c r="O12" s="0" t="n">
+      <c r="O12" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="P12" s="0" t="s">
+      <c r="P12" s="1" t="s">
         <v>62</v>
       </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="O8:R8"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G43"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.69"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="11"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="11"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="11"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="11"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="11"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="11"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="9"/>
+      <c r="B14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="11"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="11"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="11"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="11"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="11"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="11"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="9"/>
+      <c r="B22" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="11"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="11"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="11"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="11"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="11"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="11"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="8"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="9"/>
+      <c r="B30" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="11"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="11"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="11"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="11"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="11"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="11"/>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="9"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="11"/>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="7"/>
+      <c r="C38" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D38" s="8"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="9"/>
+      <c r="B39" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G39" s="11"/>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="11"/>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="11"/>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="11"/>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="11"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>